<commit_message>
Login to ACME System 1 OK
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShirleyHastier\Documents\UiPath\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD4EB7F-3965-4DA6-996B-30D78BEA3031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E9A029-4C94-4861-B2EC-F80339CF444F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1290" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Sha1Url</t>
-  </si>
-  <si>
     <t>http://www.sha1-online.com/</t>
   </si>
   <si>
@@ -137,7 +134,10 @@
     <t>System1_Credential</t>
   </si>
   <si>
-    <t>System1_Url</t>
+    <t>Sha1URL</t>
+  </si>
+  <si>
+    <t>System1URL</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -591,33 +591,33 @@
         <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Open SHA1Online app workflow.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShirleyHastier\Documents\UiPath\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E9A029-4C94-4861-B2EC-F80339CF444F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC41BD8-82E9-4035-9D5A-3CBCAB4697F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -134,10 +134,10 @@
     <t>System1_Credential</t>
   </si>
   <si>
-    <t>Sha1URL</t>
+    <t>System1URL</t>
   </si>
   <si>
-    <t>System1URL</t>
+    <t>SHA1URL</t>
   </si>
 </sst>
 </file>
@@ -519,15 +519,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="68.54296875" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -588,7 +588,7 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>30</v>
@@ -1627,12 +1627,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2738,12 +2738,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>